<commit_message>
start working on shrub biomass model fits
</commit_message>
<xml_diff>
--- a/from_JB/Shrub_Allometry_LUT_Jun2024.xlsx
+++ b/from_JB/Shrub_Allometry_LUT_Jun2024.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\battl\Dropbox\Shrub allometry\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kruth\Desktop\shrub_biomass\from_JB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{88DCE10B-D849-4B12-9943-9F716D7D4D87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D925CFE-46B9-41C0-A789-5C09E78B77D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2590,8 +2590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3950,7 +3950,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>

</xml_diff>